<commit_message>
Added environmental variable support for creds
</commit_message>
<xml_diff>
--- a/src/assets/wsj.xlsx
+++ b/src/assets/wsj.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -869,6 +869,190 @@
         <v>5004784258</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Oct 06, 2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3346</v>
+      </c>
+      <c r="D5" t="n">
+        <v>974</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2242</v>
+      </c>
+      <c r="F5" t="n">
+        <v>130</v>
+      </c>
+      <c r="G5" t="n">
+        <v>32</v>
+      </c>
+      <c r="H5" t="n">
+        <v>122</v>
+      </c>
+      <c r="I5" t="n">
+        <v>336249580</v>
+      </c>
+      <c r="J5" t="n">
+        <v>576118947</v>
+      </c>
+      <c r="K5" t="n">
+        <v>919538564</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M5" t="n">
+        <v>5396</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1635873706</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2625683225</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>4293189892</v>
+      </c>
+      <c r="R5" t="n">
+        <v>4878</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1713</v>
+      </c>
+      <c r="T5" t="n">
+        <v>2902</v>
+      </c>
+      <c r="U5" t="n">
+        <v>263</v>
+      </c>
+      <c r="V5" t="n">
+        <v>59</v>
+      </c>
+      <c r="W5" t="n">
+        <v>199</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>19974</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>1460424411</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>2334144952</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>4091868336</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Oct 06, 2022</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3346</v>
+      </c>
+      <c r="D6" t="n">
+        <v>974</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2242</v>
+      </c>
+      <c r="F6" t="n">
+        <v>130</v>
+      </c>
+      <c r="G6" t="n">
+        <v>32</v>
+      </c>
+      <c r="H6" t="n">
+        <v>122</v>
+      </c>
+      <c r="I6" t="n">
+        <v>336249580</v>
+      </c>
+      <c r="J6" t="n">
+        <v>576118947</v>
+      </c>
+      <c r="K6" t="n">
+        <v>919538564</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M6" t="n">
+        <v>5396</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1635873706</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2625683225</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
+        <v>4293189892</v>
+      </c>
+      <c r="R6" t="n">
+        <v>4878</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1713</v>
+      </c>
+      <c r="T6" t="n">
+        <v>2902</v>
+      </c>
+      <c r="U6" t="n">
+        <v>263</v>
+      </c>
+      <c r="V6" t="n">
+        <v>59</v>
+      </c>
+      <c r="W6" t="n">
+        <v>199</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>19974</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>1460424411</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>2334144952</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>4091868336</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more environmental variables
</commit_message>
<xml_diff>
--- a/src/assets/wsj.xlsx
+++ b/src/assets/wsj.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB6"/>
+  <dimension ref="A1:AB9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1053,6 +1053,282 @@
         <v>4091868336</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Oct 06, 2022</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3346</v>
+      </c>
+      <c r="D7" t="n">
+        <v>974</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2242</v>
+      </c>
+      <c r="F7" t="n">
+        <v>130</v>
+      </c>
+      <c r="G7" t="n">
+        <v>32</v>
+      </c>
+      <c r="H7" t="n">
+        <v>122</v>
+      </c>
+      <c r="I7" t="n">
+        <v>336249580</v>
+      </c>
+      <c r="J7" t="n">
+        <v>576118947</v>
+      </c>
+      <c r="K7" t="n">
+        <v>919538564</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M7" t="n">
+        <v>5396</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1635873706</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2625683225</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
+        <v>4293189892</v>
+      </c>
+      <c r="R7" t="n">
+        <v>4878</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1713</v>
+      </c>
+      <c r="T7" t="n">
+        <v>2902</v>
+      </c>
+      <c r="U7" t="n">
+        <v>263</v>
+      </c>
+      <c r="V7" t="n">
+        <v>59</v>
+      </c>
+      <c r="W7" t="n">
+        <v>199</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>19974</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>1460424411</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>2334144952</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>4091868336</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Oct 06, 2022</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3346</v>
+      </c>
+      <c r="D8" t="n">
+        <v>974</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2242</v>
+      </c>
+      <c r="F8" t="n">
+        <v>130</v>
+      </c>
+      <c r="G8" t="n">
+        <v>32</v>
+      </c>
+      <c r="H8" t="n">
+        <v>122</v>
+      </c>
+      <c r="I8" t="n">
+        <v>336249580</v>
+      </c>
+      <c r="J8" t="n">
+        <v>576118947</v>
+      </c>
+      <c r="K8" t="n">
+        <v>919538564</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M8" t="n">
+        <v>5396</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1635873706</v>
+      </c>
+      <c r="O8" t="n">
+        <v>2625683225</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="Q8" t="n">
+        <v>4293189892</v>
+      </c>
+      <c r="R8" t="n">
+        <v>4878</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1713</v>
+      </c>
+      <c r="T8" t="n">
+        <v>2902</v>
+      </c>
+      <c r="U8" t="n">
+        <v>263</v>
+      </c>
+      <c r="V8" t="n">
+        <v>59</v>
+      </c>
+      <c r="W8" t="n">
+        <v>199</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>19974</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>1460424411</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>2334144952</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>4091868336</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Oct 06, 2022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>3346</v>
+      </c>
+      <c r="D9" t="n">
+        <v>974</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2242</v>
+      </c>
+      <c r="F9" t="n">
+        <v>130</v>
+      </c>
+      <c r="G9" t="n">
+        <v>32</v>
+      </c>
+      <c r="H9" t="n">
+        <v>122</v>
+      </c>
+      <c r="I9" t="n">
+        <v>336249580</v>
+      </c>
+      <c r="J9" t="n">
+        <v>576118947</v>
+      </c>
+      <c r="K9" t="n">
+        <v>919538564</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M9" t="n">
+        <v>5396</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1635873706</v>
+      </c>
+      <c r="O9" t="n">
+        <v>2625683225</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="Q9" t="n">
+        <v>4293189892</v>
+      </c>
+      <c r="R9" t="n">
+        <v>4878</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1713</v>
+      </c>
+      <c r="T9" t="n">
+        <v>2902</v>
+      </c>
+      <c r="U9" t="n">
+        <v>263</v>
+      </c>
+      <c r="V9" t="n">
+        <v>59</v>
+      </c>
+      <c r="W9" t="n">
+        <v>199</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>19974</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>1460424411</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>2334144952</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>4091868336</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>